<commit_message>
adding total sum to end of column
</commit_message>
<xml_diff>
--- a/js/db_orig.xlsx
+++ b/js/db_orig.xlsx
@@ -5170,7 +5170,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -5212,9 +5212,6 @@
     </xf>
     <xf numFmtId="1" fontId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -9265,10 +9262,12 @@
       <c r="C123" t="s" s="5">
         <v>455</v>
       </c>
-      <c r="D123" s="14"/>
-      <c r="E123" s="14"/>
-      <c r="F123" s="14"/>
-      <c r="G123" s="14"/>
+      <c r="D123" s="12"/>
+      <c r="E123" s="12"/>
+      <c r="F123" s="12"/>
+      <c r="G123" t="s" s="5">
+        <v>6</v>
+      </c>
     </row>
     <row r="124" ht="18" customHeight="1">
       <c r="A124" t="s" s="5">
@@ -10446,10 +10445,12 @@
       <c r="C176" t="s" s="5">
         <v>582</v>
       </c>
-      <c r="D176" s="14"/>
-      <c r="E176" s="14"/>
-      <c r="F176" s="14"/>
-      <c r="G176" s="14"/>
+      <c r="D176" s="12"/>
+      <c r="E176" s="12"/>
+      <c r="F176" s="12"/>
+      <c r="G176" t="s" s="5">
+        <v>6</v>
+      </c>
     </row>
     <row r="177" ht="18" customHeight="1">
       <c r="A177" t="s" s="5">
@@ -15081,10 +15082,12 @@
       <c r="C381" t="s" s="5">
         <v>1268</v>
       </c>
-      <c r="D381" s="14"/>
-      <c r="E381" s="14"/>
-      <c r="F381" s="14"/>
-      <c r="G381" s="14"/>
+      <c r="D381" s="12"/>
+      <c r="E381" s="12"/>
+      <c r="F381" s="12"/>
+      <c r="G381" t="s" s="5">
+        <v>6</v>
+      </c>
     </row>
     <row r="382" ht="18" customHeight="1">
       <c r="A382" t="s" s="5">
@@ -16047,7 +16050,9 @@
       <c r="D424" s="12"/>
       <c r="E424" s="12"/>
       <c r="F424" s="12"/>
-      <c r="G424" s="14"/>
+      <c r="G424" t="s" s="5">
+        <v>6</v>
+      </c>
     </row>
     <row r="425" ht="18" customHeight="1">
       <c r="A425" t="s" s="5">
@@ -16105,10 +16110,12 @@
       <c r="C427" t="s" s="5">
         <v>1406</v>
       </c>
-      <c r="D427" s="14"/>
-      <c r="E427" s="14"/>
-      <c r="F427" s="14"/>
-      <c r="G427" s="14"/>
+      <c r="D427" s="12"/>
+      <c r="E427" s="12"/>
+      <c r="F427" s="12"/>
+      <c r="G427" t="s" s="5">
+        <v>6</v>
+      </c>
     </row>
     <row r="428" ht="18" customHeight="1">
       <c r="A428" t="s" s="5">
@@ -18028,6 +18035,101 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="6.625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="6.625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="6.625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="6.625" style="14" customWidth="1"/>
+    <col min="6" max="256" width="6.625" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.55" customHeight="1">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" ht="15.55" customHeight="1">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+    </row>
+    <row r="3" ht="15.55" customHeight="1">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" ht="15.55" customHeight="1">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" ht="15.55" customHeight="1">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" ht="15.55" customHeight="1">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" ht="15.55" customHeight="1">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" ht="15.55" customHeight="1">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" ht="15.55" customHeight="1">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" ht="15.55" customHeight="1">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -18120,99 +18222,4 @@
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="1" width="6.625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="6.625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="6.625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="6.625" style="16" customWidth="1"/>
-    <col min="6" max="256" width="6.625" style="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="15.55" customHeight="1">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" ht="15.55" customHeight="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" ht="15.55" customHeight="1">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" ht="15.55" customHeight="1">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" ht="15.55" customHeight="1">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" ht="15.55" customHeight="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" ht="15.55" customHeight="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" ht="15.55" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" ht="15.55" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" ht="15.55" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>